<commit_message>
First-cut analysis of NC, IL, & SC
</commit_message>
<xml_diff>
--- a/analysis/IL/IL2022-metrics.xlsx
+++ b/analysis/IL/IL2022-metrics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/method_eval/analysis/IL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B4C3CF-2A12-CA47-B409-1E20E88D9B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A294FD68-F366-A242-B8ED-F5E6F89695B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="6900" windowWidth="26840" windowHeight="15940" xr2:uid="{9F82D1CB-05A3-684F-9385-DF40F74D99BB}"/>
+    <workbookView xWindow="24360" yWindow="6420" windowWidth="26840" windowHeight="15940" xr2:uid="{9F82D1CB-05A3-684F-9385-DF40F74D99BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="IL2022_metrics" localSheetId="0">Sheet1!$A$1:$L$24</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{7B94490C-D6B3-C54F-AFC1-0C217764D23E}" name="IL2022-metrics" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/alecramsay/dev/method_eval/data/IL/IL2022-metrics.csv" comma="1">
+    <textPr sourceFile="/Users/alecramsay/dev/method_eval/data/IL/IL2022-metrics.csv" comma="1">
       <textFields count="12">
         <textField type="text"/>
         <textField/>
@@ -204,7 +204,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -212,16 +212,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,13 +565,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE5CE2C-55E8-1D4A-A696-088B869C75BF}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
+      <selection pane="bottomRight" activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,40 +696,40 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="6">
         <v>0.78288899999999995</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="6">
         <v>0.79778700000000002</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="6">
         <v>0.78405999999999998</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="6">
         <v>0.80142400000000003</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="6">
         <v>0.75439599999999996</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="6">
         <v>0.75858999999999999</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="6">
         <v>0.72979899999999998</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="6">
         <v>0.77100900000000006</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="6">
         <v>1.1461000000000001E-2</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="6">
         <v>1.188E-2</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="6">
         <v>1.036559</v>
       </c>
     </row>
@@ -862,344 +887,344 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="4">
-        <v>-27.316002999999998</v>
+        <v>-2.9332E-2</v>
       </c>
       <c r="C9" s="4">
-        <v>-33.856498999999999</v>
+        <v>-4.1054E-2</v>
       </c>
       <c r="D9" s="4">
-        <v>-30.206417999999999</v>
+        <v>-3.5437000000000003E-2</v>
       </c>
       <c r="E9" s="4">
-        <v>-31.061053999999999</v>
+        <v>-3.6263999999999998E-2</v>
       </c>
       <c r="F9" s="4">
-        <v>-11.190721999999999</v>
+        <v>1.0596E-2</v>
       </c>
       <c r="G9" s="4">
-        <v>-15.109211</v>
+        <v>1.5599999999999999E-2</v>
       </c>
       <c r="H9" s="4">
-        <v>-18.491578000000001</v>
+        <v>-2.5083999999999999E-2</v>
       </c>
       <c r="I9" s="4">
-        <v>-23.319247000000001</v>
+        <v>-1.8606999999999999E-2</v>
       </c>
       <c r="J9" s="4">
-        <v>3.899635</v>
+        <v>1.0269E-2</v>
       </c>
       <c r="K9" s="4">
-        <v>-3.996756</v>
+        <v>-1.0725E-2</v>
       </c>
       <c r="L9" s="4">
-        <v>-1.024905</v>
+        <v>-1.044405</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="4">
-        <v>-2.9332E-2</v>
+        <v>-0.119517</v>
       </c>
       <c r="C10" s="4">
-        <v>-4.1054E-2</v>
+        <v>-0.124607</v>
       </c>
       <c r="D10" s="4">
-        <v>-3.5437000000000003E-2</v>
+        <v>-0.103658</v>
       </c>
       <c r="E10" s="4">
-        <v>-3.6263999999999998E-2</v>
+        <v>-0.13012599999999999</v>
       </c>
       <c r="F10" s="4">
-        <v>1.0596E-2</v>
+        <v>-9.5044000000000003E-2</v>
       </c>
       <c r="G10" s="4">
-        <v>1.5599999999999999E-2</v>
+        <v>-9.0412000000000006E-2</v>
       </c>
       <c r="H10" s="4">
-        <v>-2.5083999999999999E-2</v>
+        <v>-0.107027</v>
       </c>
       <c r="I10" s="4">
-        <v>-1.8606999999999999E-2</v>
+        <v>-0.10847900000000001</v>
       </c>
       <c r="J10" s="4">
-        <v>1.0269E-2</v>
+        <v>6.483E-3</v>
       </c>
       <c r="K10" s="4">
-        <v>-1.0725E-2</v>
+        <v>-1.1037999999999999E-2</v>
       </c>
       <c r="L10" s="4">
-        <v>-1.044405</v>
+        <v>-1.702607</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4">
-        <v>-0.119517</v>
+        <v>-2.9315999999999998E-2</v>
       </c>
       <c r="C11" s="4">
-        <v>-0.124607</v>
+        <v>-2.4271999999999998E-2</v>
       </c>
       <c r="D11" s="4">
-        <v>-0.103658</v>
+        <v>-2.7979E-2</v>
       </c>
       <c r="E11" s="4">
-        <v>-0.13012599999999999</v>
+        <v>-3.0495000000000001E-2</v>
       </c>
       <c r="F11" s="4">
-        <v>-9.5044000000000003E-2</v>
+        <v>-5.8129999999999996E-3</v>
       </c>
       <c r="G11" s="4">
-        <v>-9.0412000000000006E-2</v>
+        <v>-4.6880000000000003E-3</v>
       </c>
       <c r="H11" s="4">
-        <v>-0.107027</v>
+        <v>-4.3833999999999998E-2</v>
       </c>
       <c r="I11" s="4">
-        <v>-0.10847900000000001</v>
+        <v>-2.2846999999999999E-2</v>
       </c>
       <c r="J11" s="4">
-        <v>6.483E-3</v>
+        <v>6.1840000000000003E-3</v>
       </c>
       <c r="K11" s="4">
-        <v>-1.1037999999999999E-2</v>
+        <v>-6.4689999999999999E-3</v>
       </c>
       <c r="L11" s="4">
-        <v>-1.702607</v>
+        <v>-1.046087</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4">
-        <v>-2.9315999999999998E-2</v>
+        <v>-0.20120299999999999</v>
       </c>
       <c r="C12" s="4">
-        <v>-2.4271999999999998E-2</v>
+        <v>-0.211197</v>
       </c>
       <c r="D12" s="4">
-        <v>-2.7979E-2</v>
+        <v>-0.193859</v>
       </c>
       <c r="E12" s="4">
-        <v>-3.0495000000000001E-2</v>
+        <v>-0.21577499999999999</v>
       </c>
       <c r="F12" s="4">
-        <v>-5.8129999999999996E-3</v>
+        <v>-0.17471999999999999</v>
       </c>
       <c r="G12" s="4">
-        <v>-4.6880000000000003E-3</v>
+        <v>-0.17450099999999999</v>
       </c>
       <c r="H12" s="4">
-        <v>-4.3833999999999998E-2</v>
+        <v>-0.16841300000000001</v>
       </c>
       <c r="I12" s="4">
-        <v>-2.2846999999999999E-2</v>
+        <v>-0.189744</v>
       </c>
       <c r="J12" s="4">
-        <v>6.1840000000000003E-3</v>
+        <v>8.3020000000000004E-3</v>
       </c>
       <c r="K12" s="4">
-        <v>-6.4689999999999999E-3</v>
+        <v>-1.1459E-2</v>
       </c>
       <c r="L12" s="4">
-        <v>-1.046087</v>
+        <v>-1.3802700000000001</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4">
-        <v>-0.20120299999999999</v>
+        <v>1.4576E-2</v>
       </c>
       <c r="C13" s="4">
-        <v>-0.211197</v>
+        <v>8.0800000000000004E-3</v>
       </c>
       <c r="D13" s="4">
-        <v>-0.193859</v>
+        <v>6.5209999999999999E-3</v>
       </c>
       <c r="E13" s="4">
-        <v>-0.21577499999999999</v>
+        <v>4.6340000000000001E-3</v>
       </c>
       <c r="F13" s="4">
-        <v>-0.17471999999999999</v>
+        <v>2.2423999999999999E-2</v>
       </c>
       <c r="G13" s="4">
-        <v>-0.17450099999999999</v>
+        <v>3.3033E-2</v>
       </c>
       <c r="H13" s="4">
-        <v>-0.16841300000000001</v>
+        <v>1.4213999999999999E-2</v>
       </c>
       <c r="I13" s="4">
-        <v>-0.189744</v>
+        <v>1.4818E-2</v>
       </c>
       <c r="J13" s="4">
-        <v>8.3020000000000004E-3</v>
+        <v>4.5019999999999999E-3</v>
       </c>
       <c r="K13" s="4">
-        <v>-1.1459E-2</v>
+        <v>-2.42E-4</v>
       </c>
       <c r="L13" s="4">
-        <v>-1.3802700000000001</v>
+        <v>-5.3754000000000003E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B14" s="4">
-        <v>1.4576E-2</v>
+        <v>2.3347E-2</v>
       </c>
       <c r="C14" s="4">
-        <v>8.0800000000000004E-3</v>
+        <v>1.6917999999999999E-2</v>
       </c>
       <c r="D14" s="4">
-        <v>6.5209999999999999E-3</v>
+        <v>1.5257E-2</v>
       </c>
       <c r="E14" s="4">
-        <v>4.6340000000000001E-3</v>
+        <v>1.7815000000000001E-2</v>
       </c>
       <c r="F14" s="4">
-        <v>2.2423999999999999E-2</v>
+        <v>2.9534999999999999E-2</v>
       </c>
       <c r="G14" s="4">
-        <v>3.3033E-2</v>
+        <v>3.8092000000000001E-2</v>
       </c>
       <c r="H14" s="4">
-        <v>1.4213999999999999E-2</v>
+        <v>2.2523000000000001E-2</v>
       </c>
       <c r="I14" s="4">
-        <v>1.4818E-2</v>
+        <v>2.3356999999999999E-2</v>
       </c>
       <c r="J14" s="4">
-        <v>4.5019999999999999E-3</v>
+        <v>3.6229999999999999E-3</v>
       </c>
       <c r="K14" s="4">
-        <v>-2.42E-4</v>
+        <v>-1.0000000000000001E-5</v>
       </c>
       <c r="L14" s="4">
-        <v>-5.3754000000000003E-2</v>
+        <v>-2.7599999999999999E-3</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2.7865000000000001E-2</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1.064E-2</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2.1849E-2</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2.6983E-2</v>
+      </c>
+      <c r="F15" s="4">
+        <v>6.4306000000000002E-2</v>
+      </c>
+      <c r="G15" s="4">
+        <v>5.7508999999999998E-2</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2.6807000000000001E-2</v>
+      </c>
+      <c r="I15" s="4">
+        <v>3.4681999999999998E-2</v>
+      </c>
+      <c r="J15" s="4">
+        <v>8.685E-3</v>
+      </c>
+      <c r="K15" s="4">
+        <v>-6.8170000000000001E-3</v>
+      </c>
+      <c r="L15" s="4">
+        <v>-0.78491699999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B16" s="6">
         <v>-8.7709999999999993E-3</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C16" s="6">
         <v>-8.8380000000000004E-3</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D16" s="6">
         <v>-8.7360000000000007E-3</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E16" s="6">
         <v>-1.3181E-2</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F16" s="6">
         <v>-7.1110000000000001E-3</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G16" s="6">
         <v>-5.0590000000000001E-3</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H16" s="6">
         <v>-8.3090000000000004E-3</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I16" s="6">
         <v>-8.5389999999999997E-3</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J16" s="6">
         <v>1.0939999999999999E-3</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K16" s="6">
         <v>-2.32E-4</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L16" s="6">
         <v>-0.212066</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="4">
-        <v>2.3347E-2</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1.6917999999999999E-2</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1.5257E-2</v>
-      </c>
-      <c r="E16" s="4">
-        <v>1.7815000000000001E-2</v>
-      </c>
-      <c r="F16" s="4">
-        <v>2.9534999999999999E-2</v>
-      </c>
-      <c r="G16" s="4">
-        <v>3.8092000000000001E-2</v>
-      </c>
-      <c r="H16" s="4">
-        <v>2.2523000000000001E-2</v>
-      </c>
-      <c r="I16" s="4">
-        <v>2.3356999999999999E-2</v>
-      </c>
-      <c r="J16" s="4">
-        <v>3.6229999999999999E-3</v>
-      </c>
-      <c r="K16" s="4">
-        <v>-1.0000000000000001E-5</v>
-      </c>
-      <c r="L16" s="4">
-        <v>-2.7599999999999999E-3</v>
-      </c>
-    </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="4">
-        <v>2.7865000000000001E-2</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1.064E-2</v>
-      </c>
-      <c r="D17" s="4">
-        <v>2.1849E-2</v>
-      </c>
-      <c r="E17" s="4">
-        <v>2.6983E-2</v>
-      </c>
-      <c r="F17" s="4">
-        <v>6.4306000000000002E-2</v>
-      </c>
-      <c r="G17" s="4">
-        <v>5.7508999999999998E-2</v>
-      </c>
-      <c r="H17" s="4">
-        <v>2.6807000000000001E-2</v>
-      </c>
-      <c r="I17" s="4">
-        <v>3.4681999999999998E-2</v>
-      </c>
-      <c r="J17" s="4">
-        <v>8.685E-3</v>
-      </c>
-      <c r="K17" s="4">
-        <v>-6.8170000000000001E-3</v>
-      </c>
-      <c r="L17" s="4">
-        <v>-0.78491699999999998</v>
+      <c r="A17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="8">
+        <v>-27.316002999999998</v>
+      </c>
+      <c r="C17" s="8">
+        <v>-33.856498999999999</v>
+      </c>
+      <c r="D17" s="8">
+        <v>-30.206417999999999</v>
+      </c>
+      <c r="E17" s="8">
+        <v>-31.061053999999999</v>
+      </c>
+      <c r="F17" s="8">
+        <v>-11.190721999999999</v>
+      </c>
+      <c r="G17" s="8">
+        <v>-15.109211</v>
+      </c>
+      <c r="H17" s="8">
+        <v>-18.491578000000001</v>
+      </c>
+      <c r="I17" s="8">
+        <v>-23.319247000000001</v>
+      </c>
+      <c r="J17" s="8">
+        <v>3.899635</v>
+      </c>
+      <c r="K17" s="8">
+        <v>-3.996756</v>
+      </c>
+      <c r="L17" s="8">
+        <v>-1.024905</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1466,6 +1491,11 @@
       </c>
       <c r="L24" s="4">
         <v>1.0893120000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L28" s="9">
+        <v>5.5999999999999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IL re-worked along with a guide
</commit_message>
<xml_diff>
--- a/analysis/IL/IL2022-metrics.xlsx
+++ b/analysis/IL/IL2022-metrics.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/method_eval/analysis/IL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55EAF1E-57AF-6E4E-9EB7-1C6254E53D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AB727C-3E44-4543-8B75-BEDBE1668C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14900" yWindow="9400" windowWidth="26860" windowHeight="16440" xr2:uid="{DE8FCAD4-7CE8-134D-982D-78CBA55338E8}"/>
+    <workbookView xWindow="18680" yWindow="5700" windowWidth="26860" windowHeight="16440" xr2:uid="{DE8FCAD4-7CE8-134D-982D-78CBA55338E8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId1"/>
+    <sheet name="Vf" sheetId="2" r:id="rId2"/>
+    <sheet name="Sf" sheetId="3" r:id="rId3"/>
+    <sheet name="Decl" sheetId="5" r:id="rId4"/>
+    <sheet name="Responsiveness" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="IL2022_metrics" localSheetId="0">Sheet1!$A$1:$L$34</definedName>
+    <definedName name="IL2022_metrics" localSheetId="0">All!$A$1:$L$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
   <si>
     <t>METRIC</t>
   </si>
@@ -193,10 +197,13 @@
     <t>Δ/SEM</t>
   </si>
   <si>
-    <t>Average for bias measures</t>
-  </si>
-  <si>
     <t>except declination</t>
+  </si>
+  <si>
+    <t>RSE</t>
+  </si>
+  <si>
+    <t>Average for unit measures</t>
   </si>
 </sst>
 </file>
@@ -206,7 +213,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -222,6 +229,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,7 +253,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -257,11 +279,146 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -275,9 +432,18 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,13 +762,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA32DA68-AB04-824C-9C2A-7891B8690AD0}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomRight" activeCell="L13" sqref="A1:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,9 +777,10 @@
     <col min="2" max="9" width="9.83203125" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -651,8 +818,11 @@
         <v>42</v>
       </c>
       <c r="M1" s="4"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O1" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -689,8 +859,12 @@
       <c r="L2" s="6">
         <v>9.9880999999999998E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O2" s="6">
+        <f>J2/I2</f>
+        <v>7.251425769657557E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
@@ -728,8 +902,9 @@
         <v>1.036559</v>
       </c>
       <c r="M3" s="9"/>
-    </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O3" s="8"/>
+    </row>
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -766,8 +941,9 @@
       <c r="L4" s="6">
         <v>1.0364949999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -804,8 +980,9 @@
       <c r="L5" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="O5" s="6"/>
+    </row>
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -842,8 +1019,9 @@
       <c r="L6" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -880,8 +1058,9 @@
       <c r="L7" s="6">
         <v>-1.702607</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
@@ -919,8 +1098,9 @@
         <v>-1.3802700000000001</v>
       </c>
       <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O8" s="8"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -957,8 +1137,9 @@
       <c r="L9" s="6">
         <v>-0.216838</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -995,47 +1176,48 @@
       <c r="L10" s="6">
         <v>-0.166105</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="6">
         <v>-2.9315999999999998E-2</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="6">
         <v>-2.4271999999999998E-2</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="6">
         <v>-2.7979E-2</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="6">
         <v>-3.0495000000000001E-2</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="6">
         <v>-5.8129999999999996E-3</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="6">
         <v>-4.6880000000000003E-3</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="6">
         <v>-4.3833999999999998E-2</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="6">
         <v>-2.2846999999999999E-2</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="6">
         <v>6.1840000000000003E-3</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="6">
         <v>-6.4689999999999999E-3</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="6">
         <v>-1.046087</v>
       </c>
-      <c r="M11" s="13"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
@@ -1073,8 +1255,9 @@
         <v>-1.044405</v>
       </c>
       <c r="M12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O12" s="8"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1111,8 +1294,9 @@
       <c r="L13" s="6">
         <v>-1.024905</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1149,8 +1333,9 @@
       <c r="L14" s="6">
         <v>-5.3754000000000003E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1187,8 +1372,9 @@
       <c r="L15" s="6">
         <v>-0.212066</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1225,8 +1411,9 @@
       <c r="L16" s="6">
         <v>-2.7599999999999999E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>26</v>
       </c>
@@ -1264,8 +1451,9 @@
         <v>-0.78491699999999998</v>
       </c>
       <c r="M17" s="9"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O17" s="8"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1302,8 +1490,9 @@
       <c r="L18" s="6">
         <v>1.045264</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1340,8 +1529,9 @@
       <c r="L19" s="6">
         <v>-0.67378099999999996</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O19" s="6"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>29</v>
       </c>
@@ -1379,11 +1569,12 @@
         <v>-0.84468900000000002</v>
       </c>
       <c r="M20" s="9"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O20" s="8"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1421,7 +1612,7 @@
         <v>1.036559</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -1459,7 +1650,7 @@
         <v>1.0364679999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1497,7 +1688,7 @@
         <v>1.0364679999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -1535,7 +1726,7 @@
         <v>0.52217800000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
@@ -1573,10 +1764,10 @@
         <v>0.11914</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
@@ -1614,7 +1805,7 @@
         <v>0.232737</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
@@ -1652,10 +1843,10 @@
         <v>-0.24490200000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1693,7 +1884,7 @@
         <v>0.190967</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -1809,7 +2000,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I36" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J36" s="6">
         <f>AVERAGE(J7:J12,J14,J17)</f>
@@ -1826,10 +2017,433 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I37" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CDA771-991A-6647-BD89-B43EF59E6145}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="12" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0.58169999999999999</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0.58660000000000001</v>
+      </c>
+      <c r="D2" s="15">
+        <v>0.59019999999999995</v>
+      </c>
+      <c r="E2" s="15">
+        <v>0.58560000000000001</v>
+      </c>
+      <c r="F2" s="15">
+        <v>0.57969999999999999</v>
+      </c>
+      <c r="G2" s="15">
+        <v>0.58409999999999995</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0.56140000000000001</v>
+      </c>
+      <c r="I2" s="15">
+        <v>0.58130000000000004</v>
+      </c>
+      <c r="J2" s="15">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="K2" s="15">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="L2" s="16">
+        <v>9.9900000000000003E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DC6109-6ED7-C24A-8C85-FACBBE9C7259}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="12" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0.78290000000000004</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0.79779999999999995</v>
+      </c>
+      <c r="D2" s="15">
+        <v>0.78410000000000002</v>
+      </c>
+      <c r="E2" s="15">
+        <v>0.8014</v>
+      </c>
+      <c r="F2" s="15">
+        <v>0.75439999999999996</v>
+      </c>
+      <c r="G2" s="15">
+        <v>0.75860000000000005</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0.7298</v>
+      </c>
+      <c r="I2" s="15">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="J2" s="15">
+        <v>1.15E-2</v>
+      </c>
+      <c r="K2" s="15">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="L2" s="16">
+        <v>1.0366</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1677BD89-91AE-724C-911E-0B3C89C62CDE}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="A2:L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="9" width="8.83203125" customWidth="1"/>
+    <col min="10" max="12" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="15">
+        <v>-27.316002999999998</v>
+      </c>
+      <c r="C2" s="15">
+        <v>-33.856498999999999</v>
+      </c>
+      <c r="D2" s="15">
+        <v>-30.206417999999999</v>
+      </c>
+      <c r="E2" s="15">
+        <v>-31.061053999999999</v>
+      </c>
+      <c r="F2" s="15">
+        <v>-11.190721999999999</v>
+      </c>
+      <c r="G2" s="15">
+        <v>-15.109211</v>
+      </c>
+      <c r="H2" s="15">
+        <v>-18.491578000000001</v>
+      </c>
+      <c r="I2" s="15">
+        <v>-23.319247000000001</v>
+      </c>
+      <c r="J2" s="15">
+        <v>3.899635</v>
+      </c>
+      <c r="K2" s="15">
+        <v>-3.996756</v>
+      </c>
+      <c r="L2" s="16">
+        <v>-1.024905</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A769BF-7DC4-C749-9144-D584A315BB97}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="12" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="17">
+        <v>3.46313</v>
+      </c>
+      <c r="C2" s="17">
+        <v>3.4390480000000001</v>
+      </c>
+      <c r="D2" s="17">
+        <v>3.1491929999999999</v>
+      </c>
+      <c r="E2" s="17">
+        <v>3.5192939999999999</v>
+      </c>
+      <c r="F2" s="17">
+        <v>3.192882</v>
+      </c>
+      <c r="G2" s="17">
+        <v>3.0751949999999999</v>
+      </c>
+      <c r="H2" s="17">
+        <v>3.7435049999999999</v>
+      </c>
+      <c r="I2" s="17">
+        <v>3.353186</v>
+      </c>
+      <c r="J2" s="17">
+        <v>0.105183</v>
+      </c>
+      <c r="K2" s="17">
+        <v>0.109944</v>
+      </c>
+      <c r="L2" s="19">
+        <v>1.045264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="21">
+        <v>1.7084630000000001</v>
+      </c>
+      <c r="C3" s="21">
+        <v>1.1841330000000001</v>
+      </c>
+      <c r="D3" s="21">
+        <v>1.649149</v>
+      </c>
+      <c r="E3" s="21">
+        <v>1.078962</v>
+      </c>
+      <c r="F3" s="21">
+        <v>2.377005</v>
+      </c>
+      <c r="G3" s="21">
+        <v>2.2119219999999999</v>
+      </c>
+      <c r="H3" s="21">
+        <v>2.963419</v>
+      </c>
+      <c r="I3" s="21">
+        <v>1.910765</v>
+      </c>
+      <c r="J3" s="21">
+        <v>0.30024899999999999</v>
+      </c>
+      <c r="K3" s="21">
+        <v>-0.20230200000000001</v>
+      </c>
+      <c r="L3" s="22">
+        <v>-0.67378099999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>